<commit_message>
factor(tests_for_factorise) : add TestDeleteItems
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_doublons.xlsx
+++ b/fichiers_xls/test_doublons.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -68,7 +68,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -91,7 +90,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -102,15 +101,6 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -129,9 +119,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,499 +383,499 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="8.550000000000001" customWidth="1" style="7" min="1" max="8"/>
+    <col width="8.550000000000001" customWidth="1" style="4" min="1" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="8">
-      <c r="A1" s="9" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Nom</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Prénom</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Adresse de courriel</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>État</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="G1" s="9" t="n"/>
-      <c r="H1" s="10" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="8">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="G1" s="6" t="n"/>
+      <c r="H1" s="7" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Aatif Mieulet</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Paola</t>
         </is>
       </c>
-      <c r="C2" s="9" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D2" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="G2" s="9" t="n"/>
-      <c r="H2" s="10" t="n"/>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="G2" s="6" t="n"/>
+      <c r="H2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="C3" s="9" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="10" t="n"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="8">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Abdel Moneim</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G4" s="9" t="n"/>
-      <c r="H4" s="10" t="n"/>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="8">
-      <c r="A5" s="9" t="inlineStr">
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" s="7" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Abdelali</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
       </c>
-      <c r="F5" s="9" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="n"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="8">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" s="7" t="n"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Abdallah</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="C6" s="11" t="inlineStr">
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="F6" s="8" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G6" s="11" t="n"/>
-      <c r="H6" s="12" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="8">
-      <c r="A7" s="9" t="inlineStr">
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="5">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Abdelgow</t>
         </is>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
       </c>
-      <c r="F7" s="9" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="10" t="n"/>
-    </row>
-    <row r="8" ht="15" customHeight="1" s="8">
-      <c r="A8" s="9" t="inlineStr">
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="5">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Abdelhadi</t>
         </is>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Nouh</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
       </c>
-      <c r="F8" s="9" t="inlineStr">
+      <c r="F8" s="6" t="inlineStr">
         <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="10" t="n"/>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="8">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="G8" s="6" t="n"/>
+      <c r="H8" s="7" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="5">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Abdenbaoui</t>
         </is>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
       </c>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G9" s="9" t="n"/>
-      <c r="H9" s="10" t="n"/>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="8">
-      <c r="A10" s="9" t="inlineStr">
+      <c r="G9" s="6" t="n"/>
+      <c r="H9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="5">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Abdulhoussen</t>
         </is>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>Houzefa</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
       </c>
-      <c r="F10" s="9" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G10" s="9" t="n"/>
-      <c r="H10" s="10" t="n"/>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="8">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="G10" s="6" t="n"/>
+      <c r="H10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="5">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>Abed Meraim</t>
         </is>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Zakaria</t>
         </is>
       </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>20221641@etud.univ-evry.fr</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="6" t="inlineStr">
         <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="G11" s="9" t="n"/>
-      <c r="H11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1" s="8">
-      <c r="A12" s="9" t="inlineStr">
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" s="6" t="n"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1" s="5">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G12" s="9" t="n"/>
-      <c r="H12" s="9" t="n"/>
-    </row>
-    <row r="13" ht="15" customHeight="1" s="8">
-      <c r="A13" s="9" t="inlineStr">
+      <c r="G12" s="6" t="n"/>
+      <c r="H12" s="6" t="n"/>
+    </row>
+    <row r="13" ht="15" customHeight="1" s="5">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B13" s="9" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
       </c>
-      <c r="F13" s="9" t="inlineStr">
+      <c r="F13" s="6" t="inlineStr">
         <is>
           <t>6,72</t>
         </is>
       </c>
-      <c r="G13" s="9" t="n"/>
-      <c r="H13" s="9" t="n"/>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="8">
-      <c r="A14" s="11" t="inlineStr">
+      <c r="G13" s="6" t="n"/>
+      <c r="H13" s="6" t="n"/>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="5">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Abdelkarim</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="C14" s="11" t="inlineStr">
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="F14" s="11" t="inlineStr">
+      <c r="F14" s="8" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G14" s="13" t="n"/>
-      <c r="H14" s="13" t="n"/>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="8">
-      <c r="B15" s="7">
+      <c r="G14" s="10" t="n"/>
+      <c r="H14" s="10" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="5">
+      <c r="B15" s="4">
         <f>F13+F14</f>
         <v/>
       </c>
     </row>
-    <row r="16" ht="13.5" customHeight="1" s="8"/>
-    <row r="17" ht="13.5" customHeight="1" s="8"/>
+    <row r="16" ht="13.5" customHeight="1" s="5"/>
+    <row r="17" ht="13.5" customHeight="1" s="5"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -904,498 +892,498 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="8.550000000000001" customWidth="1" style="7" min="1" max="8"/>
+    <col width="8.550000000000001" customWidth="1" style="4" min="1" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="8">
-      <c r="A1" s="9" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Nom</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Prénom</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Adresse de courriel</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>État</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="G1" s="9" t="n"/>
-      <c r="H1" s="10" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="8">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="G1" s="6" t="n"/>
+      <c r="H1" s="7" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Aatif Mieulet</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Paola</t>
         </is>
       </c>
-      <c r="C2" s="9" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D2" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="G2" s="9" t="n"/>
-      <c r="H2" s="10" t="n"/>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="G2" s="6" t="n"/>
+      <c r="H2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="C3" s="9" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="10" t="n"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="8">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Abdel Moneim</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G4" s="9" t="n"/>
-      <c r="H4" s="10" t="n"/>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="8">
-      <c r="A5" s="9" t="inlineStr">
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" s="7" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Abdelali</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
       </c>
-      <c r="F5" s="9" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="n"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="8">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" s="7" t="n"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Abdallah</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="C6" s="11" t="inlineStr">
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="F6" s="8" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G6" s="11" t="n"/>
-      <c r="H6" s="12" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="8">
-      <c r="A7" s="9" t="inlineStr">
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="5">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Abdelgow</t>
         </is>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
       </c>
-      <c r="F7" s="9" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="10" t="n"/>
-    </row>
-    <row r="8" ht="15" customHeight="1" s="8">
-      <c r="A8" s="9" t="inlineStr">
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="5">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Abdelhadi</t>
         </is>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Nouh</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
       </c>
-      <c r="F8" s="9" t="inlineStr">
+      <c r="F8" s="6" t="inlineStr">
         <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="10" t="n"/>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="8">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="G8" s="6" t="n"/>
+      <c r="H8" s="7" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="5">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Abdenbaoui</t>
         </is>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
       </c>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G9" s="9" t="n"/>
-      <c r="H9" s="10" t="n"/>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="8">
-      <c r="A10" s="9" t="inlineStr">
+      <c r="G9" s="6" t="n"/>
+      <c r="H9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="5">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Abdulhoussen</t>
         </is>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>Houzefa</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
       </c>
-      <c r="F10" s="9" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G10" s="9" t="n"/>
-      <c r="H10" s="10" t="n"/>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="8">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="G10" s="6" t="n"/>
+      <c r="H10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="5">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>Abed Meraim</t>
         </is>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Zakaria</t>
         </is>
       </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>20221641@etud.univ-evry.fr</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="6" t="inlineStr">
         <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="G11" s="9" t="n"/>
-      <c r="H11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1" s="8">
-      <c r="A12" s="9" t="inlineStr">
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" s="6" t="n"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1" s="5">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G12" s="9" t="n"/>
-      <c r="H12" s="9" t="n"/>
-    </row>
-    <row r="13" ht="15" customHeight="1" s="8">
-      <c r="A13" s="9" t="inlineStr">
+      <c r="G12" s="6" t="n"/>
+      <c r="H12" s="6" t="n"/>
+    </row>
+    <row r="13" ht="15" customHeight="1" s="5">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B13" s="9" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
       </c>
-      <c r="F13" s="9" t="inlineStr">
+      <c r="F13" s="6" t="inlineStr">
         <is>
           <t>6,72</t>
         </is>
       </c>
-      <c r="G13" s="9" t="n"/>
-      <c r="H13" s="9" t="n"/>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="8">
-      <c r="A14" s="11" t="inlineStr">
+      <c r="G13" s="6" t="n"/>
+      <c r="H13" s="6" t="n"/>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="5">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Abdelkarim</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="C14" s="11" t="inlineStr">
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="F14" s="11" t="inlineStr">
+      <c r="F14" s="8" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G14" s="13" t="n"/>
-      <c r="H14" s="13" t="n"/>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="8">
-      <c r="B15" s="7">
+      <c r="G14" s="10" t="n"/>
+      <c r="H14" s="10" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="5">
+      <c r="B15" s="4">
         <f>F13+F14</f>
         <v/>
       </c>
     </row>
-    <row r="16" ht="13.5" customHeight="1" s="8"/>
-    <row r="17" ht="13.5" customHeight="1" s="8"/>
+    <row r="16" ht="13.5" customHeight="1" s="5"/>
+    <row r="17" ht="13.5" customHeight="1" s="5"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1420,498 +1408,498 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="8.550000000000001" customWidth="1" style="7" min="1" max="8"/>
+    <col width="8.550000000000001" customWidth="1" style="4" min="1" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="8">
-      <c r="A1" s="9" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Nom</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Prénom</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Adresse de courriel</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>État</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="G1" s="9" t="n"/>
-      <c r="H1" s="10" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="8">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="G1" s="6" t="n"/>
+      <c r="H1" s="7" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Aatif Mieulet</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Paola</t>
         </is>
       </c>
-      <c r="C2" s="9" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D2" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="G2" s="9" t="n"/>
-      <c r="H2" s="10" t="n"/>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="G2" s="6" t="n"/>
+      <c r="H2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="C3" s="9" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="10" t="n"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="8">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Abdel Moneim</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G4" s="9" t="n"/>
-      <c r="H4" s="10" t="n"/>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="8">
-      <c r="A5" s="9" t="inlineStr">
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" s="7" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Abdelali</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
       </c>
-      <c r="F5" s="9" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="n"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="8">
-      <c r="A6" s="11" t="inlineStr">
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" s="7" t="n"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>Abdallah</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="C6" s="11" t="inlineStr">
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D6" s="11" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E6" s="11" t="inlineStr">
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="F6" s="11" t="inlineStr">
+      <c r="F6" s="8" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G6" s="11" t="n"/>
-      <c r="H6" s="12" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="8">
-      <c r="A7" s="9" t="inlineStr">
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="9" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="5">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Abdelgow</t>
         </is>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
       </c>
-      <c r="F7" s="9" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="10" t="n"/>
-    </row>
-    <row r="8" ht="15" customHeight="1" s="8">
-      <c r="A8" s="9" t="inlineStr">
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="5">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Abdelhadi</t>
         </is>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Nouh</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
       </c>
-      <c r="F8" s="9" t="inlineStr">
+      <c r="F8" s="6" t="inlineStr">
         <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="10" t="n"/>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="8">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="G8" s="6" t="n"/>
+      <c r="H8" s="7" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="5">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Abdenbaoui</t>
         </is>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
       </c>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G9" s="9" t="n"/>
-      <c r="H9" s="10" t="n"/>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="8">
-      <c r="A10" s="9" t="inlineStr">
+      <c r="G9" s="6" t="n"/>
+      <c r="H9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="5">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Abdulhoussen</t>
         </is>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>Houzefa</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
       </c>
-      <c r="F10" s="9" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G10" s="9" t="n"/>
-      <c r="H10" s="10" t="n"/>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="8">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="G10" s="6" t="n"/>
+      <c r="H10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="5">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>Abed Meraim</t>
         </is>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Zakaria</t>
         </is>
       </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>20221641@etud.univ-evry.fr</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="6" t="inlineStr">
         <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="G11" s="9" t="n"/>
-      <c r="H11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1" s="8">
-      <c r="A12" s="9" t="inlineStr">
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" s="6" t="n"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1" s="5">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G12" s="9" t="n"/>
-      <c r="H12" s="9" t="n"/>
-    </row>
-    <row r="13" ht="15" customHeight="1" s="8">
-      <c r="A13" s="9" t="inlineStr">
+      <c r="G12" s="6" t="n"/>
+      <c r="H12" s="6" t="n"/>
+    </row>
+    <row r="13" ht="15" customHeight="1" s="5">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B13" s="9" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
       </c>
-      <c r="F13" s="9" t="inlineStr">
+      <c r="F13" s="6" t="inlineStr">
         <is>
           <t>6,72</t>
         </is>
       </c>
-      <c r="G13" s="9" t="n"/>
-      <c r="H13" s="9" t="n"/>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="8">
-      <c r="A14" s="11" t="inlineStr">
+      <c r="G13" s="6" t="n"/>
+      <c r="H13" s="6" t="n"/>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="5">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>Abdelkarim</t>
         </is>
       </c>
-      <c r="B14" s="11" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="C14" s="11" t="inlineStr">
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="11" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr">
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="F14" s="11" t="inlineStr">
+      <c r="F14" s="8" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G14" s="13" t="n"/>
-      <c r="H14" s="13" t="n"/>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="8">
-      <c r="B15" s="7">
+      <c r="G14" s="10" t="n"/>
+      <c r="H14" s="10" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="5">
+      <c r="B15" s="4">
         <f>F13+F14</f>
         <v/>
       </c>
     </row>
-    <row r="16" ht="13.5" customHeight="1" s="8"/>
-    <row r="17" ht="13.5" customHeight="1" s="8"/>
+    <row r="16" ht="13.5" customHeight="1" s="5"/>
+    <row r="17" ht="13.5" customHeight="1" s="5"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1935,502 +1923,502 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="8">
-      <c r="A1" s="9" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Nom</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Prénom</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Adresse de courriel</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>État</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="G1" s="9" t="n"/>
-      <c r="H1" s="10" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="8">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="G1" s="6" t="n"/>
+      <c r="H1" s="7" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Aatif Mieulet</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Paola</t>
         </is>
       </c>
-      <c r="C2" s="9" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D2" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="G2" s="9" t="n"/>
-      <c r="H2" s="10" t="n"/>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="G2" s="6" t="n"/>
+      <c r="H2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="C3" s="9" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="10" t="n"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="8">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Abdel Moneim</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G4" s="9" t="n"/>
-      <c r="H4" s="10" t="n"/>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="8">
-      <c r="A5" s="9" t="inlineStr">
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" s="7" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Abdelali</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
       </c>
-      <c r="F5" s="9" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="n"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="8">
-      <c r="A6" s="9" t="inlineStr">
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" s="7" t="n"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Abdallah</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="F6" s="9" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G6" s="9" t="n"/>
-      <c r="H6" s="10" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="8">
-      <c r="A7" s="9" t="inlineStr">
+      <c r="G6" s="6" t="n"/>
+      <c r="H6" s="7" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="5">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Abdelgow</t>
         </is>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
       </c>
-      <c r="F7" s="9" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="10" t="n"/>
-    </row>
-    <row r="8" ht="15" customHeight="1" s="8">
-      <c r="A8" s="9" t="inlineStr">
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="5">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Abdelhadi</t>
         </is>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Nouh</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
       </c>
-      <c r="F8" s="9" t="inlineStr">
+      <c r="F8" s="6" t="inlineStr">
         <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="10" t="n"/>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="8">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="G8" s="6" t="n"/>
+      <c r="H8" s="7" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="5">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Abdenbaoui</t>
         </is>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
       </c>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G9" s="9" t="n"/>
-      <c r="H9" s="10" t="n"/>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="8">
-      <c r="A10" s="9" t="inlineStr">
+      <c r="G9" s="6" t="n"/>
+      <c r="H9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="5">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Abdulhoussen</t>
         </is>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>Houzefa</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
       </c>
-      <c r="F10" s="9" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G10" s="9" t="n"/>
-      <c r="H10" s="10" t="n"/>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="8">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="G10" s="6" t="n"/>
+      <c r="H10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="5">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>Abed Meraim</t>
         </is>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Zakaria</t>
         </is>
       </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>20221641@etud.univ-evry.fr</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="6" t="inlineStr">
         <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="G11" s="9" t="n"/>
-      <c r="H11" s="9" t="n"/>
-    </row>
-    <row r="12" ht="15" customHeight="1" s="8">
-      <c r="A12" s="9" t="inlineStr">
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" s="6" t="n"/>
+    </row>
+    <row r="12" ht="15" customHeight="1" s="5">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G12" s="9" t="n"/>
-      <c r="H12" s="9" t="n"/>
-    </row>
-    <row r="13" ht="15" customHeight="1" s="8">
-      <c r="A13" s="9" t="inlineStr">
+      <c r="G12" s="6" t="n"/>
+      <c r="H12" s="6" t="n"/>
+    </row>
+    <row r="13" ht="15" customHeight="1" s="5">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B13" s="9" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
       </c>
-      <c r="F13" s="9" t="inlineStr">
+      <c r="F13" s="6" t="inlineStr">
         <is>
           <t>6,72</t>
         </is>
       </c>
-      <c r="G13" s="9" t="n"/>
-      <c r="H13" s="9" t="n"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1" s="8">
-      <c r="A14" s="9" t="inlineStr">
+      <c r="G13" s="6" t="n"/>
+      <c r="H13" s="6" t="n"/>
+    </row>
+    <row r="14" ht="13.5" customHeight="1" s="5">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>Abdelkarim</t>
         </is>
       </c>
-      <c r="B14" s="9" t="inlineStr">
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="C14" s="9" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="F14" s="9" t="inlineStr">
+      <c r="F14" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" s="8">
-      <c r="B15" s="7">
+    <row r="15" ht="15" customHeight="1" s="5">
+      <c r="B15" s="4">
         <f>F13+F14</f>
         <v/>
       </c>
     </row>
-    <row r="1048567" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048568" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048569" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048570" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048571" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048572" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048573" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048574" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048575" ht="12.75" customHeight="1" s="8"/>
-    <row r="1048576" ht="12.75" customHeight="1" s="8"/>
+    <row r="1048567" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048568" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048569" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048570" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048571" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048572" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048573" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048574" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048575" ht="12.75" customHeight="1" s="5"/>
+    <row r="1048576" ht="12.75" customHeight="1" s="5"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2447,556 +2435,556 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="8.550000000000001" customWidth="1" style="7" min="1" max="8"/>
+    <col width="8.550000000000001" customWidth="1" style="4" min="1" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="8">
-      <c r="A1" s="9" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>Nom</t>
         </is>
       </c>
-      <c r="B1" s="9" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Prénom</t>
         </is>
       </c>
-      <c r="C1" s="9" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Adresse de courriel</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>État</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="G1" s="9" t="n"/>
-      <c r="H1" s="10" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1" s="8">
-      <c r="A2" s="9" t="inlineStr">
+      <c r="G1" s="6" t="n"/>
+      <c r="H1" s="7" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Aatif Mieulet</t>
         </is>
       </c>
-      <c r="B2" s="9" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Paola</t>
         </is>
       </c>
-      <c r="C2" s="9" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D2" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E2" s="9" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
       </c>
-      <c r="F2" s="9" t="inlineStr">
+      <c r="F2" s="6" t="inlineStr">
         <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="G2" s="9" t="n"/>
-      <c r="H2" s="10" t="n"/>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="8">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="G2" s="6" t="n"/>
+      <c r="H2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
       </c>
-      <c r="B3" s="9" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="C3" s="9" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D3" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
       </c>
-      <c r="F3" s="9" t="inlineStr">
+      <c r="F3" s="6" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="G3" s="9" t="n"/>
-      <c r="H3" s="10" t="n"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="8">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="G3" s="6" t="n"/>
+      <c r="H3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Abdel Moneim</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
+      <c r="B4" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
       </c>
-      <c r="F4" s="9" t="inlineStr">
+      <c r="F4" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G4" s="9" t="n"/>
-      <c r="H4" s="10" t="n"/>
-    </row>
-    <row r="5" ht="15" customHeight="1" s="8">
-      <c r="A5" s="9" t="inlineStr">
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" s="7" t="n"/>
+    </row>
+    <row r="5" ht="15" customHeight="1" s="5">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Abdallah</t>
         </is>
       </c>
-      <c r="B5" s="9" t="inlineStr">
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="F5" s="9" t="inlineStr">
+      <c r="F5" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="10" t="n"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="8">
-      <c r="A6" s="9" t="inlineStr">
+      <c r="G5" s="6" t="n"/>
+      <c r="H5" s="7" t="n"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Abdelali</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="6" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
       </c>
-      <c r="F6" s="9" t="inlineStr">
+      <c r="F6" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G6" s="9" t="n"/>
-      <c r="H6" s="10" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="8">
-      <c r="A7" s="9" t="inlineStr">
+      <c r="G6" s="6" t="n"/>
+      <c r="H6" s="7" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="5">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Abdallah</t>
         </is>
       </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="F7" s="9" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G7" s="9" t="n"/>
-      <c r="H7" s="10" t="n"/>
-    </row>
-    <row r="8" ht="15" customHeight="1" s="8">
-      <c r="A8" s="9" t="inlineStr">
+      <c r="G7" s="6" t="n"/>
+      <c r="H7" s="7" t="n"/>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="5">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Abdelgow</t>
         </is>
       </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B8" s="6" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
       </c>
-      <c r="F8" s="9" t="inlineStr">
+      <c r="F8" s="6" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="G8" s="9" t="n"/>
-      <c r="H8" s="10" t="n"/>
-    </row>
-    <row r="9" ht="15" customHeight="1" s="8">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="G8" s="6" t="n"/>
+      <c r="H8" s="7" t="n"/>
+    </row>
+    <row r="9" ht="15" customHeight="1" s="5">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Abdelhadi</t>
         </is>
       </c>
-      <c r="B9" s="9" t="inlineStr">
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>Nouh</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
       </c>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="6" t="inlineStr">
         <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="G9" s="9" t="n"/>
-      <c r="H9" s="10" t="n"/>
-    </row>
-    <row r="10" ht="15" customHeight="1" s="8">
-      <c r="A10" s="9" t="inlineStr">
+      <c r="G9" s="6" t="n"/>
+      <c r="H9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="5">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Abdenbaoui</t>
         </is>
       </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
       </c>
-      <c r="F10" s="9" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G10" s="9" t="n"/>
-      <c r="H10" s="10" t="n"/>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="8">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="G10" s="6" t="n"/>
+      <c r="H10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="5">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>Abdulhoussen</t>
         </is>
       </c>
-      <c r="B11" s="9" t="inlineStr">
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Houzefa</t>
         </is>
       </c>
-      <c r="C11" s="9" t="inlineStr">
+      <c r="C11" s="6" t="inlineStr">
         <is>
           <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E11" s="6" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
       </c>
-      <c r="F11" s="9" t="inlineStr">
+      <c r="F11" s="6" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G11" s="9" t="n"/>
-      <c r="H11" s="10" t="n"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1" s="8">
-      <c r="A12" s="9" t="inlineStr">
+      <c r="G11" s="6" t="n"/>
+      <c r="H11" s="7" t="n"/>
+    </row>
+    <row r="12" ht="13.5" customHeight="1" s="5">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>Abdelkarim</t>
         </is>
       </c>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C12" s="6" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D12" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E12" s="9" t="inlineStr">
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="F12" s="9" t="inlineStr">
+      <c r="F12" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" s="8">
-      <c r="A13" s="9" t="inlineStr">
+    <row r="13" ht="15" customHeight="1" s="5">
+      <c r="A13" s="6" t="inlineStr">
         <is>
           <t>Abed Meraim</t>
         </is>
       </c>
-      <c r="B13" s="9" t="inlineStr">
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>Zakaria</t>
         </is>
       </c>
-      <c r="C13" s="9" t="inlineStr">
+      <c r="C13" s="6" t="inlineStr">
         <is>
           <t>20221641@etud.univ-evry.fr</t>
         </is>
       </c>
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E13" s="9" t="inlineStr">
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
       </c>
-      <c r="F13" s="9" t="inlineStr">
+      <c r="F13" s="6" t="inlineStr">
         <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="G13" s="9" t="n"/>
-      <c r="H13" s="9" t="n"/>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="8">
-      <c r="A14" s="9" t="inlineStr">
+      <c r="G13" s="6" t="n"/>
+      <c r="H13" s="6" t="n"/>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="5">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B14" s="9" t="inlineStr">
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="C14" s="9" t="inlineStr">
+      <c r="C14" s="6" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E14" s="9" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
       </c>
-      <c r="F14" s="9" t="inlineStr">
+      <c r="F14" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G14" s="9" t="n"/>
-      <c r="H14" s="9" t="n"/>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="8">
-      <c r="A15" s="9" t="inlineStr">
+      <c r="G14" s="6" t="n"/>
+      <c r="H14" s="6" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="5">
+      <c r="A15" s="6" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B15" s="9" t="inlineStr">
+      <c r="B15" s="6" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="C15" s="9" t="inlineStr">
+      <c r="C15" s="6" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D15" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E15" s="9" t="inlineStr">
+      <c r="D15" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
       </c>
-      <c r="F15" s="9" t="inlineStr">
+      <c r="F15" s="6" t="inlineStr">
         <is>
           <t>6,72</t>
         </is>
       </c>
-      <c r="G15" s="9" t="n"/>
-      <c r="H15" s="9" t="n"/>
-    </row>
-    <row r="16" ht="13.5" customHeight="1" s="8">
-      <c r="A16" s="9" t="inlineStr">
+      <c r="G15" s="6" t="n"/>
+      <c r="H15" s="6" t="n"/>
+    </row>
+    <row r="16" ht="13.5" customHeight="1" s="5">
+      <c r="A16" s="6" t="inlineStr">
         <is>
           <t>Abdelkarim</t>
         </is>
       </c>
-      <c r="B16" s="9" t="inlineStr">
+      <c r="B16" s="6" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="C16" s="9" t="inlineStr">
+      <c r="C16" s="6" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D16" s="9" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="E16" s="9" t="inlineStr">
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="F16" s="9" t="inlineStr">
+      <c r="F16" s="6" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="13.5" customHeight="1" s="8">
-      <c r="B17" s="7">
+    <row r="17" ht="13.5" customHeight="1" s="5">
+      <c r="B17" s="4">
         <f>F15+F16</f>
         <v/>
       </c>

</xml_diff>